<commit_message>
ajout anciennes données df (et résolution d'erreurs d'import)
</commit_message>
<xml_diff>
--- a/assets/HistoriqueCTI_BJ.xlsx
+++ b/assets/HistoriqueCTI_BJ.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Affaires_generales\Indicateurs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41445c22dc8dedf8/Bureau/Télécom SudParis/S8/Cassiopée/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_4DAE21EAA085A9A3BEAC20D8C5EA500F65404FAF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FF82E82-C432-406E-BE96-4328E63BE8C7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -44,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,13 +128,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,16 +415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2021</v>
       </c>
@@ -428,7 +441,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +461,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,7 +481,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -488,7 +501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -508,7 +521,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -520,6 +533,12 @@
       </c>
       <c r="D7" s="3">
         <v>828</v>
+      </c>
+      <c r="E7" s="4">
+        <v>833</v>
+      </c>
+      <c r="F7" s="4">
+        <v>821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>